<commit_message>
Add PersistanceConfig so that the repo can read/write to multiple places, i.e. file or DB.
</commit_message>
<xml_diff>
--- a/src/test/resources/temp.xlsx
+++ b/src/test/resources/temp.xlsx
@@ -388,4 +388,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml>
+</file>
+
+<file path=xl/worksheets/sheet8.xml>
+</file>
+
+<file path=xl/worksheets/sheet9.xml>
 </file>
</xml_diff>